<commit_message>
added latest of 1/3
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640C71B0-4C30-4A19-B365-35EB2C64B4C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B5ADE2-C6FA-4C25-AE35-902106AF53DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="132" windowWidth="19560" windowHeight="12168" activeTab="2" xr2:uid="{C553E39C-A1CD-49FC-A10F-9B2CFF840EDB}"/>
+    <workbookView xWindow="1200" yWindow="2016" windowWidth="19692" windowHeight="11544" activeTab="2" xr2:uid="{C553E39C-A1CD-49FC-A10F-9B2CFF840EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Standings" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>Random Seed</t>
   </si>
@@ -237,6 +238,90 @@
   </si>
   <si>
     <t>Column13</t>
+  </si>
+  <si>
+    <t>Column122</t>
+  </si>
+  <si>
+    <t>Column123</t>
+  </si>
+  <si>
+    <t>Column124</t>
+  </si>
+  <si>
+    <t>Column125</t>
+  </si>
+  <si>
+    <t>Column126</t>
+  </si>
+  <si>
+    <t>Column1222</t>
+  </si>
+  <si>
+    <t>Column1223</t>
+  </si>
+  <si>
+    <t>Column1224</t>
+  </si>
+  <si>
+    <t>Column1225</t>
+  </si>
+  <si>
+    <t>Column14</t>
+  </si>
+  <si>
+    <t>Column132</t>
+  </si>
+  <si>
+    <t>Column133</t>
+  </si>
+  <si>
+    <t>Column1322</t>
+  </si>
+  <si>
+    <t>Column1323</t>
+  </si>
+  <si>
+    <t>Column1324</t>
+  </si>
+  <si>
+    <t>Column1325</t>
+  </si>
+  <si>
+    <t>Column1326</t>
+  </si>
+  <si>
+    <t>Column13252</t>
+  </si>
+  <si>
+    <t>Column13253</t>
+  </si>
+  <si>
+    <t>Column13254</t>
+  </si>
+  <si>
+    <t>Column13255</t>
+  </si>
+  <si>
+    <t>Column13256</t>
+  </si>
+  <si>
+    <t>Column13257</t>
+  </si>
+  <si>
+    <t>Column13258</t>
+  </si>
+  <si>
+    <t>Column13259</t>
+  </si>
+  <si>
+    <t>Column132510</t>
+  </si>
+  <si>
+    <t>Column132511</t>
+  </si>
+  <si>
+    <t>Column132512</t>
   </si>
 </sst>
 </file>
@@ -317,7 +402,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="50">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -488,7 +657,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Bingo Rakings</a:t>
+              <a:t>Bingo Rankings</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -609,16 +778,16 @@
                   <c:v>David</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Steph</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Mike</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>Jan</c:v>
+                  <c:v>Devon</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Devon</c:v>
+                  <c:v>Mike</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Marcus</c:v>
@@ -634,45 +803,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Standings!$S$2:$S$15</c:f>
+              <c:f>Standings!$AU$2:$AU$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
@@ -1449,16 +1618,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>397328</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1504,51 +1673,79 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A88997B-32EA-4C65-9C12-24CC25834524}" name="Table134" displayName="Table134" ref="B1:D19" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A88997B-32EA-4C65-9C12-24CC25834524}" name="Table134" displayName="Table134" ref="B1:D19" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="B1:D19" xr:uid="{210C98D4-9E1B-4933-8C3D-53E8404172C4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D19">
     <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F0EE673-9B26-4BD1-B5CE-799EF9DB1FBC}" name="40" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{4F0EE673-9B26-4BD1-B5CE-799EF9DB1FBC}" name="40" dataDxfId="47">
       <calculatedColumnFormula>RAND()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9A64CAE0-D0F5-4B2C-893B-28EF4C574AAF}" name="Amount" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{63454A59-667A-4C48-8D2B-C8AFD0912497}" name="Exercise" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{9A64CAE0-D0F5-4B2C-893B-28EF4C574AAF}" name="Amount" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{63454A59-667A-4C48-8D2B-C8AFD0912497}" name="Exercise" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6953A8DC-D2D7-4099-955A-911AC8C68F58}" name="Table2" displayName="Table2" ref="A1:S16" totalsRowCount="1">
-  <autoFilter ref="A1:S15" xr:uid="{515B8832-AA46-422C-BABE-AC8057912BB1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S15">
-    <sortCondition descending="1" ref="S1:S15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6953A8DC-D2D7-4099-955A-911AC8C68F58}" name="Table2" displayName="Table2" ref="A1:AU16" totalsRowCount="1">
+  <autoFilter ref="A1:AU15" xr:uid="{515B8832-AA46-422C-BABE-AC8057912BB1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU15">
+    <sortCondition descending="1" ref="AU1:AU15"/>
   </sortState>
-  <tableColumns count="19">
+  <tableColumns count="47">
     <tableColumn id="1" xr3:uid="{4D5E04F8-62DC-47B7-BEA3-B2D4890F9EA5}" name="Name"/>
     <tableColumn id="2" xr3:uid="{65152ACF-91A6-467A-A50B-EDF21C68B622}" name="Initial"/>
-    <tableColumn id="3" xr3:uid="{71FF741F-AC35-4B4D-88F4-3D39C72130C9}" name="Column1" totalsRowLabel="9/3/2020" totalsRowDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{A0F92D98-6CEE-4A8C-BA04-3475B86B34FD}" name="Column2" totalsRowLabel="9/8/2020" totalsRowDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{5B158799-89BA-48BB-B710-00CCDC09A2B1}" name="Column3" totalsRowDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{AF44A75A-6403-49BB-96FC-17AF67B68884}" name="Column4" totalsRowDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{528A9CD5-25F2-421B-AF7B-FD99BF2AF5E3}" name="Column5" totalsRowDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{D5C20C53-4C98-4D77-B3B2-0A81DFE35E48}" name="Column6" totalsRowDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{B2AAFD2A-3802-40A9-A658-FE344C71F9B3}" name="Column7" totalsRowDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{76A030F4-747D-460F-B0BA-904B64A77F85}" name="Column8" totalsRowDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{9BF23289-E6ED-423D-936C-23C867337FDD}" name="Column9" totalsRowFunction="custom" totalsRowDxfId="7">
+    <tableColumn id="3" xr3:uid="{71FF741F-AC35-4B4D-88F4-3D39C72130C9}" name="Column1" totalsRowLabel="9/3/2020" totalsRowDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{A0F92D98-6CEE-4A8C-BA04-3475B86B34FD}" name="Column2" totalsRowLabel="9/8/2020" totalsRowDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{5B158799-89BA-48BB-B710-00CCDC09A2B1}" name="Column3" totalsRowDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{AF44A75A-6403-49BB-96FC-17AF67B68884}" name="Column4" totalsRowDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{528A9CD5-25F2-421B-AF7B-FD99BF2AF5E3}" name="Column5" totalsRowDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{D5C20C53-4C98-4D77-B3B2-0A81DFE35E48}" name="Column6" totalsRowDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{B2AAFD2A-3802-40A9-A658-FE344C71F9B3}" name="Column7" totalsRowDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{76A030F4-747D-460F-B0BA-904B64A77F85}" name="Column8" totalsRowDxfId="36"/>
+    <tableColumn id="14" xr3:uid="{9BF23289-E6ED-423D-936C-23C867337FDD}" name="Column9" totalsRowFunction="custom" totalsRowDxfId="35">
       <totalsRowFormula>"9/24/2020"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F95B0867-2A69-4B55-BB96-D3B53881818C}" name="Column92" totalsRowDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{8B9DF6A0-087E-4DEE-B91C-698B58F5D1DC}" name="Column10" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{DD2CC6B0-5810-4BF1-9C39-3CAC2C465A09}" name="Column22" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{5B625666-1E70-4A73-B974-7E6342DBEC01}" name="Don't Use" totalsRowDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{1E4DA5DD-E520-4467-B62E-D35BCB55F1B8}" name="Column11" totalsRowDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{A45FC7C4-B068-4D1D-9C8C-4196BB5F9684}" name="Column12" totalsRowDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{C941376A-2872-4A6A-8248-B3066F1389F8}" name="Column13" totalsRowDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{4AB274B9-0A1B-4F26-A207-E5383510846D}" name="Total" dataDxfId="16">
-      <calculatedColumnFormula>SUM(B2:R2)</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{F95B0867-2A69-4B55-BB96-D3B53881818C}" name="Column92" totalsRowDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{8B9DF6A0-087E-4DEE-B91C-698B58F5D1DC}" name="Column10" totalsRowDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{DD2CC6B0-5810-4BF1-9C39-3CAC2C465A09}" name="Column22" totalsRowDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{5B625666-1E70-4A73-B974-7E6342DBEC01}" name="Don't Use" totalsRowDxfId="31"/>
+    <tableColumn id="17" xr3:uid="{1E4DA5DD-E520-4467-B62E-D35BCB55F1B8}" name="Column11" totalsRowDxfId="30"/>
+    <tableColumn id="18" xr3:uid="{A45FC7C4-B068-4D1D-9C8C-4196BB5F9684}" name="Column12" totalsRowDxfId="29"/>
+    <tableColumn id="20" xr3:uid="{48F0508F-463E-43CA-8C85-49293EC49BF4}" name="Column122" totalsRowDxfId="28"/>
+    <tableColumn id="25" xr3:uid="{43A690BF-1E5D-4A05-AA37-5D0776C2A4DF}" name="Column1222" totalsRowDxfId="27"/>
+    <tableColumn id="26" xr3:uid="{CB955D0B-F820-49B2-8EC9-C283F677CAA9}" name="Column1223" totalsRowDxfId="26"/>
+    <tableColumn id="27" xr3:uid="{19EEBD25-E6B7-4468-A267-E3C62392334F}" name="Column1224" totalsRowDxfId="25"/>
+    <tableColumn id="28" xr3:uid="{6FDF1F57-2C4D-4330-AC1E-701F4EF1D3B2}" name="Column1225" totalsRowDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{5D63798E-7BF2-4D18-9097-13BB25358CB0}" name="Column123" totalsRowDxfId="23"/>
+    <tableColumn id="21" xr3:uid="{1A7AEBD5-3314-432C-85D3-9ED0F238D773}" name="Column124" totalsRowDxfId="22"/>
+    <tableColumn id="22" xr3:uid="{FC7A65DE-AB69-4822-B851-60E02F47CB74}" name="Column125" totalsRowDxfId="21"/>
+    <tableColumn id="24" xr3:uid="{B5EF7674-A2E2-441D-8520-589F30506002}" name="Column126" totalsRowDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{C941376A-2872-4A6A-8248-B3066F1389F8}" name="Column13" totalsRowDxfId="19"/>
+    <tableColumn id="30" xr3:uid="{CCAC5527-345A-4C55-9D44-AB79EF39A1BF}" name="Column132" totalsRowDxfId="18"/>
+    <tableColumn id="38" xr3:uid="{ED0390A5-6A70-4F6A-91F5-FE84A8B9E1DB}" name="Column1325" totalsRowDxfId="17"/>
+    <tableColumn id="47" xr3:uid="{4431CC4B-4ED0-4ABC-924C-91BF103A20AE}" name="Column132512" totalsRowDxfId="0"/>
+    <tableColumn id="46" xr3:uid="{6C437A0E-8A6D-4478-B7E2-0A34778B60E7}" name="Column132511" totalsRowDxfId="16"/>
+    <tableColumn id="45" xr3:uid="{9A3DF020-9578-41BA-B496-F936693A989C}" name="Column132510" totalsRowDxfId="15"/>
+    <tableColumn id="44" xr3:uid="{BC2BA275-E6CB-4DA6-8F45-9CBE680057DA}" name="Column13259" totalsRowDxfId="14"/>
+    <tableColumn id="43" xr3:uid="{35E6A8F6-ED8E-4399-825F-596EA5967F1B}" name="Column13258" totalsRowDxfId="13"/>
+    <tableColumn id="42" xr3:uid="{5104C125-2E27-4387-B9D2-F39CC14AA704}" name="Column13257" totalsRowDxfId="12"/>
+    <tableColumn id="41" xr3:uid="{8D85446A-EE97-4F1E-A08E-CC3234DCCC71}" name="Column13256" totalsRowDxfId="11"/>
+    <tableColumn id="36" xr3:uid="{786E475F-C29F-4717-950D-2E6F33ECFF47}" name="Column13255" totalsRowDxfId="10"/>
+    <tableColumn id="35" xr3:uid="{D88C32B8-F96F-492C-A956-BB09A5B161B4}" name="Column13254" totalsRowDxfId="9"/>
+    <tableColumn id="40" xr3:uid="{51BFE2E5-CC91-403A-BF9F-767E63AB3B5F}" name="Column13253" totalsRowDxfId="8"/>
+    <tableColumn id="39" xr3:uid="{668EFE9F-6816-497C-AD65-FC3F61DB685F}" name="Column13252" totalsRowDxfId="7"/>
+    <tableColumn id="37" xr3:uid="{51F3C527-95E4-43EC-873A-CE8762E66373}" name="Column1326" totalsRowDxfId="6"/>
+    <tableColumn id="34" xr3:uid="{45998420-A149-48F7-AAC3-A0986EE61766}" name="Column1324" totalsRowDxfId="5"/>
+    <tableColumn id="33" xr3:uid="{2350E26F-CFDD-4C66-9FA4-222BE61750EC}" name="Column1323" totalsRowDxfId="4"/>
+    <tableColumn id="32" xr3:uid="{AF9F6D68-11AD-4EDC-97A2-6B8422EF708A}" name="Column1322" totalsRowDxfId="3"/>
+    <tableColumn id="31" xr3:uid="{7DAB08F1-69BD-435F-9829-3DA19CC651F9}" name="Column133" totalsRowDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{8AB5D6A3-9A8A-414C-9097-C57CEA5E3BD4}" name="Column14" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4AB274B9-0A1B-4F26-A207-E5383510846D}" name="Total" dataDxfId="44">
+      <calculatedColumnFormula>SUM(B2:AT2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1885,7 +2082,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B18" ca="1" si="0">RAND()</f>
-        <v>0.29420354368043411</v>
+        <v>0.13693444198846549</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -1901,7 +2098,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68052361934166483</v>
+        <v>0.32777126153350888</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -1917,7 +2114,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41189656616263803</v>
+        <v>0.57640585361891561</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -1930,7 +2127,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42114950643877869</v>
+        <v>0.5888910308344395</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1946,7 +2143,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3201624180785263</v>
+        <v>0.175022611561365</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -1962,7 +2159,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2894862665559188E-2</v>
+        <v>5.4993682245761732E-2</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1978,7 +2175,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88121508932779224</v>
+        <v>0.45326993594414999</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -1994,7 +2191,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68396378322730222</v>
+        <v>0.98000093612082251</v>
       </c>
       <c r="C9">
         <v>80</v>
@@ -2010,7 +2207,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84357036339642655</v>
+        <v>0.71975956677636921</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -2026,7 +2223,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13729651026549428</v>
+        <v>0.2901195514184719</v>
       </c>
       <c r="C11">
         <v>40</v>
@@ -2042,7 +2239,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8584453824943612</v>
+        <v>0.56434000247051175</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -2058,7 +2255,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71510364870376841</v>
+        <v>0.18921517907222851</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -2074,7 +2271,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94591461068040594</v>
+        <v>0.86817487514601865</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -2090,7 +2287,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56127978645097765</v>
+        <v>0.96718836812319808</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -2106,7 +2303,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69763820887885364</v>
+        <v>5.1325429360683517E-2</v>
       </c>
       <c r="C16">
         <v>25</v>
@@ -2122,7 +2319,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47956873691400959</v>
+        <v>6.9496635513224159E-2</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2137,7 +2334,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91869082395793022</v>
+        <v>0.87959809618146656</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
@@ -2155,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62829EA8-433C-4970-81C0-C08ED68590D1}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2186,14 +2383,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:B19" ca="1" si="0">RAND()</f>
-        <v>0.41793284837035827</v>
+        <f ca="1">RAND()</f>
+        <v>0.64629800926414294</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
@@ -2202,238 +2399,238 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.92882034363820276</v>
+        <f ca="1">RAND()</f>
+        <v>0.40265585760391598</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A17" si="1">A3+1</f>
+        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.38433640793530022</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
+        <f ca="1">RAND()</f>
+        <v>0.59831229335687275</v>
+      </c>
+      <c r="C4" s="4">
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42558482707638701</v>
+        <f ca="1">RAND()</f>
+        <v>0.59555341970490006</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.18783938685117019</v>
+        <f ca="1">RAND()</f>
+        <v>0.52600230817636118</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8824574040185893</v>
+        <f ca="1">RAND()</f>
+        <v>0.55637418142846817</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.99868703928935187</v>
+        <f ca="1">RAND()</f>
+        <v>0.20819407311893579</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.0332923026581784E-2</v>
+        <f ca="1">RAND()</f>
+        <v>0.91595403892067884</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43700296740149136</v>
+        <f ca="1">RAND()</f>
+        <v>0.73810449310557458</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.90393841433918465</v>
+        <f ca="1">RAND()</f>
+        <v>0.78125316430626557</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.63064708844750494</v>
-      </c>
-      <c r="C12" s="4">
-        <v>25</v>
+        <f ca="1">RAND()</f>
+        <v>0.1986318843469258</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.20406719089470937</v>
+        <f ca="1">RAND()</f>
+        <v>0.11266898390639346</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.9077460674229449E-3</v>
+        <f ca="1">RAND()</f>
+        <v>0.90091416573345129</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.84833803852341982</v>
+        <f ca="1">RAND()</f>
+        <v>0.94717527321635697</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.60522315203197707</v>
+        <f ca="1">RAND()</f>
+        <v>0.45889841765492723</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.33788202720427474</v>
+        <f ca="1">RAND()</f>
+        <v>0.1725431620145782</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
@@ -2441,14 +2638,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.70275103363432667</v>
+        <f ca="1">RAND()</f>
+        <v>0.72206491682041718</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
@@ -2456,14 +2653,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.24893856670377779</v>
+        <f ca="1">RAND()</f>
+        <v>0.90018485183687569</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2478,19 +2675,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1535E-8E4E-497C-81C7-403374733E7F}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:AU16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="15" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="16" max="18" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="29" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="10.44140625" customWidth="1"/>
+    <col min="31" max="46" width="10.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2543,13 +2742,97 @@
         <v>68</v>
       </c>
       <c r="R1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AB1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2568,12 +2851,27 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="S2">
-        <f t="shared" ref="S2:S15" si="0">SUM(B2:R2)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>1</v>
+      </c>
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <v>1</v>
+      </c>
+      <c r="AU2">
+        <f>SUM(B2:AT2)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2604,12 +2902,42 @@
       <c r="R3">
         <v>1</v>
       </c>
-      <c r="S3">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>2</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
+        <f>SUM(B3:AT3)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2631,12 +2959,42 @@
       <c r="Q4">
         <v>1</v>
       </c>
-      <c r="S4">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AP4">
+        <v>1</v>
+      </c>
+      <c r="AR4">
+        <v>2</v>
+      </c>
+      <c r="AS4">
+        <v>1</v>
+      </c>
+      <c r="AT4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
+        <f>SUM(B4:AT4)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2649,15 +3007,42 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
       <c r="S5">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>2</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>2</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <f>SUM(B5:AT5)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2670,12 +3055,39 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="S6">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>2</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <f>SUM(B6:AT6)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2692,11 +3104,29 @@
         <v>1</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>2</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <f>SUM(B7:AT7)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2718,102 +3148,159 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="S8">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>2</v>
+      </c>
+      <c r="AU8">
+        <f>SUM(B8:AT8)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <f>SUM(B9:AT9)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>20</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10">
-        <v>16</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AU10">
+        <f>SUM(B10:AT10)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>18</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
       <c r="N11">
         <v>1</v>
       </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AU11">
+        <f>SUM(B11:AT11)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B12">
-        <v>18</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AU12">
+        <f>SUM(B12:AT12)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2829,36 +3316,39 @@
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="AU13">
+        <f>SUM(B13:AT13)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="S14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="AU14">
+        <f>SUM(B14:AT14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="S15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="AU15">
+        <f>SUM(B15:AT15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
         <v>55</v>
       </c>
@@ -2882,6 +3372,34 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="5"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="5"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="5"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
side leg lifts now 1.5minutes
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bingo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B5ADE2-C6FA-4C25-AE35-902106AF53DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774E114E-0CED-4CFE-A3EC-00D930629571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2016" windowWidth="19692" windowHeight="11544" activeTab="2" xr2:uid="{C553E39C-A1CD-49FC-A10F-9B2CFF840EDB}"/>
+    <workbookView xWindow="552" yWindow="804" windowWidth="19692" windowHeight="11544" activeTab="2" xr2:uid="{C553E39C-A1CD-49FC-A10F-9B2CFF840EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Standings" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="105">
   <si>
     <t>Random Seed</t>
   </si>
@@ -322,6 +321,27 @@
   </si>
   <si>
     <t>Column132512</t>
+  </si>
+  <si>
+    <t>Column132513</t>
+  </si>
+  <si>
+    <t>Column132514</t>
+  </si>
+  <si>
+    <t>Column1325132</t>
+  </si>
+  <si>
+    <t>Column15</t>
+  </si>
+  <si>
+    <t>Calf and Bicep</t>
+  </si>
+  <si>
+    <t>Horse Stance Punches</t>
+  </si>
+  <si>
+    <t>Column142</t>
   </si>
 </sst>
 </file>
@@ -389,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -398,11 +418,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="55">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -778,10 +814,10 @@
                   <c:v>David</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Jan</c:v>
+                  <c:v>Steph</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Steph</c:v>
+                  <c:v>Jan</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Devon</c:v>
@@ -803,42 +839,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Standings!$AU$2:$AU$15</c:f>
+              <c:f>Standings!$AZ$2:$AZ$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>27</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>20</c:v>
@@ -1618,13 +1654,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>47</xdr:col>
+      <xdr:col>52</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>56</xdr:col>
+      <xdr:col>61</xdr:col>
       <xdr:colOff>397328</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>174172</xdr:rowOff>
@@ -1673,79 +1709,84 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A88997B-32EA-4C65-9C12-24CC25834524}" name="Table134" displayName="Table134" ref="B1:D19" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="B1:D19" xr:uid="{210C98D4-9E1B-4933-8C3D-53E8404172C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A88997B-32EA-4C65-9C12-24CC25834524}" name="Table134" displayName="Table134" ref="B1:D21" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+  <autoFilter ref="B1:D21" xr:uid="{210C98D4-9E1B-4933-8C3D-53E8404172C4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D19">
-    <sortCondition ref="B1:B19"/>
+    <sortCondition descending="1" ref="B1:B19"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4F0EE673-9B26-4BD1-B5CE-799EF9DB1FBC}" name="40" dataDxfId="47">
+    <tableColumn id="1" xr3:uid="{4F0EE673-9B26-4BD1-B5CE-799EF9DB1FBC}" name="40" dataDxfId="52">
       <calculatedColumnFormula>RAND()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9A64CAE0-D0F5-4B2C-893B-28EF4C574AAF}" name="Amount" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{63454A59-667A-4C48-8D2B-C8AFD0912497}" name="Exercise" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{9A64CAE0-D0F5-4B2C-893B-28EF4C574AAF}" name="Amount" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{63454A59-667A-4C48-8D2B-C8AFD0912497}" name="Exercise" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6953A8DC-D2D7-4099-955A-911AC8C68F58}" name="Table2" displayName="Table2" ref="A1:AU16" totalsRowCount="1">
-  <autoFilter ref="A1:AU15" xr:uid="{515B8832-AA46-422C-BABE-AC8057912BB1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU15">
-    <sortCondition descending="1" ref="AU1:AU15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6953A8DC-D2D7-4099-955A-911AC8C68F58}" name="Table2" displayName="Table2" ref="A1:AZ16" totalsRowCount="1">
+  <autoFilter ref="A1:AZ15" xr:uid="{515B8832-AA46-422C-BABE-AC8057912BB1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AZ15">
+    <sortCondition descending="1" ref="AZ1:AZ15"/>
   </sortState>
-  <tableColumns count="47">
+  <tableColumns count="52">
     <tableColumn id="1" xr3:uid="{4D5E04F8-62DC-47B7-BEA3-B2D4890F9EA5}" name="Name"/>
     <tableColumn id="2" xr3:uid="{65152ACF-91A6-467A-A50B-EDF21C68B622}" name="Initial"/>
-    <tableColumn id="3" xr3:uid="{71FF741F-AC35-4B4D-88F4-3D39C72130C9}" name="Column1" totalsRowLabel="9/3/2020" totalsRowDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{A0F92D98-6CEE-4A8C-BA04-3475B86B34FD}" name="Column2" totalsRowLabel="9/8/2020" totalsRowDxfId="42"/>
-    <tableColumn id="8" xr3:uid="{5B158799-89BA-48BB-B710-00CCDC09A2B1}" name="Column3" totalsRowDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{AF44A75A-6403-49BB-96FC-17AF67B68884}" name="Column4" totalsRowDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{528A9CD5-25F2-421B-AF7B-FD99BF2AF5E3}" name="Column5" totalsRowDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{D5C20C53-4C98-4D77-B3B2-0A81DFE35E48}" name="Column6" totalsRowDxfId="38"/>
-    <tableColumn id="12" xr3:uid="{B2AAFD2A-3802-40A9-A658-FE344C71F9B3}" name="Column7" totalsRowDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{76A030F4-747D-460F-B0BA-904B64A77F85}" name="Column8" totalsRowDxfId="36"/>
-    <tableColumn id="14" xr3:uid="{9BF23289-E6ED-423D-936C-23C867337FDD}" name="Column9" totalsRowFunction="custom" totalsRowDxfId="35">
+    <tableColumn id="3" xr3:uid="{71FF741F-AC35-4B4D-88F4-3D39C72130C9}" name="Column1" totalsRowLabel="9/3/2020" totalsRowDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{A0F92D98-6CEE-4A8C-BA04-3475B86B34FD}" name="Column2" totalsRowLabel="9/8/2020" totalsRowDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{5B158799-89BA-48BB-B710-00CCDC09A2B1}" name="Column3" totalsRowDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{AF44A75A-6403-49BB-96FC-17AF67B68884}" name="Column4" totalsRowDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{528A9CD5-25F2-421B-AF7B-FD99BF2AF5E3}" name="Column5" totalsRowDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{D5C20C53-4C98-4D77-B3B2-0A81DFE35E48}" name="Column6" totalsRowDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{B2AAFD2A-3802-40A9-A658-FE344C71F9B3}" name="Column7" totalsRowDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{76A030F4-747D-460F-B0BA-904B64A77F85}" name="Column8" totalsRowDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{9BF23289-E6ED-423D-936C-23C867337FDD}" name="Column9" totalsRowFunction="custom" totalsRowDxfId="40">
       <totalsRowFormula>"9/24/2020"</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F95B0867-2A69-4B55-BB96-D3B53881818C}" name="Column92" totalsRowDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{8B9DF6A0-087E-4DEE-B91C-698B58F5D1DC}" name="Column10" totalsRowDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{DD2CC6B0-5810-4BF1-9C39-3CAC2C465A09}" name="Column22" totalsRowDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{5B625666-1E70-4A73-B974-7E6342DBEC01}" name="Don't Use" totalsRowDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{1E4DA5DD-E520-4467-B62E-D35BCB55F1B8}" name="Column11" totalsRowDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{A45FC7C4-B068-4D1D-9C8C-4196BB5F9684}" name="Column12" totalsRowDxfId="29"/>
-    <tableColumn id="20" xr3:uid="{48F0508F-463E-43CA-8C85-49293EC49BF4}" name="Column122" totalsRowDxfId="28"/>
-    <tableColumn id="25" xr3:uid="{43A690BF-1E5D-4A05-AA37-5D0776C2A4DF}" name="Column1222" totalsRowDxfId="27"/>
-    <tableColumn id="26" xr3:uid="{CB955D0B-F820-49B2-8EC9-C283F677CAA9}" name="Column1223" totalsRowDxfId="26"/>
-    <tableColumn id="27" xr3:uid="{19EEBD25-E6B7-4468-A267-E3C62392334F}" name="Column1224" totalsRowDxfId="25"/>
-    <tableColumn id="28" xr3:uid="{6FDF1F57-2C4D-4330-AC1E-701F4EF1D3B2}" name="Column1225" totalsRowDxfId="24"/>
-    <tableColumn id="23" xr3:uid="{5D63798E-7BF2-4D18-9097-13BB25358CB0}" name="Column123" totalsRowDxfId="23"/>
-    <tableColumn id="21" xr3:uid="{1A7AEBD5-3314-432C-85D3-9ED0F238D773}" name="Column124" totalsRowDxfId="22"/>
-    <tableColumn id="22" xr3:uid="{FC7A65DE-AB69-4822-B851-60E02F47CB74}" name="Column125" totalsRowDxfId="21"/>
-    <tableColumn id="24" xr3:uid="{B5EF7674-A2E2-441D-8520-589F30506002}" name="Column126" totalsRowDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{C941376A-2872-4A6A-8248-B3066F1389F8}" name="Column13" totalsRowDxfId="19"/>
-    <tableColumn id="30" xr3:uid="{CCAC5527-345A-4C55-9D44-AB79EF39A1BF}" name="Column132" totalsRowDxfId="18"/>
-    <tableColumn id="38" xr3:uid="{ED0390A5-6A70-4F6A-91F5-FE84A8B9E1DB}" name="Column1325" totalsRowDxfId="17"/>
-    <tableColumn id="47" xr3:uid="{4431CC4B-4ED0-4ABC-924C-91BF103A20AE}" name="Column132512" totalsRowDxfId="0"/>
-    <tableColumn id="46" xr3:uid="{6C437A0E-8A6D-4478-B7E2-0A34778B60E7}" name="Column132511" totalsRowDxfId="16"/>
-    <tableColumn id="45" xr3:uid="{9A3DF020-9578-41BA-B496-F936693A989C}" name="Column132510" totalsRowDxfId="15"/>
-    <tableColumn id="44" xr3:uid="{BC2BA275-E6CB-4DA6-8F45-9CBE680057DA}" name="Column13259" totalsRowDxfId="14"/>
-    <tableColumn id="43" xr3:uid="{35E6A8F6-ED8E-4399-825F-596EA5967F1B}" name="Column13258" totalsRowDxfId="13"/>
-    <tableColumn id="42" xr3:uid="{5104C125-2E27-4387-B9D2-F39CC14AA704}" name="Column13257" totalsRowDxfId="12"/>
-    <tableColumn id="41" xr3:uid="{8D85446A-EE97-4F1E-A08E-CC3234DCCC71}" name="Column13256" totalsRowDxfId="11"/>
-    <tableColumn id="36" xr3:uid="{786E475F-C29F-4717-950D-2E6F33ECFF47}" name="Column13255" totalsRowDxfId="10"/>
-    <tableColumn id="35" xr3:uid="{D88C32B8-F96F-492C-A956-BB09A5B161B4}" name="Column13254" totalsRowDxfId="9"/>
-    <tableColumn id="40" xr3:uid="{51BFE2E5-CC91-403A-BF9F-767E63AB3B5F}" name="Column13253" totalsRowDxfId="8"/>
-    <tableColumn id="39" xr3:uid="{668EFE9F-6816-497C-AD65-FC3F61DB685F}" name="Column13252" totalsRowDxfId="7"/>
-    <tableColumn id="37" xr3:uid="{51F3C527-95E4-43EC-873A-CE8762E66373}" name="Column1326" totalsRowDxfId="6"/>
-    <tableColumn id="34" xr3:uid="{45998420-A149-48F7-AAC3-A0986EE61766}" name="Column1324" totalsRowDxfId="5"/>
-    <tableColumn id="33" xr3:uid="{2350E26F-CFDD-4C66-9FA4-222BE61750EC}" name="Column1323" totalsRowDxfId="4"/>
-    <tableColumn id="32" xr3:uid="{AF9F6D68-11AD-4EDC-97A2-6B8422EF708A}" name="Column1322" totalsRowDxfId="3"/>
-    <tableColumn id="31" xr3:uid="{7DAB08F1-69BD-435F-9829-3DA19CC651F9}" name="Column133" totalsRowDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{8AB5D6A3-9A8A-414C-9097-C57CEA5E3BD4}" name="Column14" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4AB274B9-0A1B-4F26-A207-E5383510846D}" name="Total" dataDxfId="44">
-      <calculatedColumnFormula>SUM(B2:AT2)</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{F95B0867-2A69-4B55-BB96-D3B53881818C}" name="Column92" totalsRowDxfId="39"/>
+    <tableColumn id="15" xr3:uid="{8B9DF6A0-087E-4DEE-B91C-698B58F5D1DC}" name="Column10" totalsRowDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{DD2CC6B0-5810-4BF1-9C39-3CAC2C465A09}" name="Column22" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{5B625666-1E70-4A73-B974-7E6342DBEC01}" name="Don't Use" totalsRowDxfId="36"/>
+    <tableColumn id="17" xr3:uid="{1E4DA5DD-E520-4467-B62E-D35BCB55F1B8}" name="Column11" totalsRowDxfId="35"/>
+    <tableColumn id="18" xr3:uid="{A45FC7C4-B068-4D1D-9C8C-4196BB5F9684}" name="Column12" totalsRowDxfId="34"/>
+    <tableColumn id="20" xr3:uid="{48F0508F-463E-43CA-8C85-49293EC49BF4}" name="Column122" totalsRowDxfId="33"/>
+    <tableColumn id="25" xr3:uid="{43A690BF-1E5D-4A05-AA37-5D0776C2A4DF}" name="Column1222" totalsRowDxfId="32"/>
+    <tableColumn id="26" xr3:uid="{CB955D0B-F820-49B2-8EC9-C283F677CAA9}" name="Column1223" totalsRowDxfId="31"/>
+    <tableColumn id="27" xr3:uid="{19EEBD25-E6B7-4468-A267-E3C62392334F}" name="Column1224" totalsRowDxfId="30"/>
+    <tableColumn id="28" xr3:uid="{6FDF1F57-2C4D-4330-AC1E-701F4EF1D3B2}" name="Column1225" totalsRowDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{5D63798E-7BF2-4D18-9097-13BB25358CB0}" name="Column123" totalsRowDxfId="28"/>
+    <tableColumn id="21" xr3:uid="{1A7AEBD5-3314-432C-85D3-9ED0F238D773}" name="Column124" totalsRowDxfId="27"/>
+    <tableColumn id="22" xr3:uid="{FC7A65DE-AB69-4822-B851-60E02F47CB74}" name="Column125" totalsRowDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{B5EF7674-A2E2-441D-8520-589F30506002}" name="Column126" totalsRowDxfId="25"/>
+    <tableColumn id="19" xr3:uid="{C941376A-2872-4A6A-8248-B3066F1389F8}" name="Column13" totalsRowDxfId="24"/>
+    <tableColumn id="30" xr3:uid="{CCAC5527-345A-4C55-9D44-AB79EF39A1BF}" name="Column132" totalsRowDxfId="23"/>
+    <tableColumn id="38" xr3:uid="{ED0390A5-6A70-4F6A-91F5-FE84A8B9E1DB}" name="Column1325" totalsRowDxfId="22"/>
+    <tableColumn id="48" xr3:uid="{F0535FD3-6ABC-4359-A328-80F94820297E}" name="Column132513" totalsRowDxfId="21"/>
+    <tableColumn id="50" xr3:uid="{5EB204DD-E3B9-4110-94FC-7C8601B936B0}" name="Column1325132" totalsRowDxfId="20"/>
+    <tableColumn id="49" xr3:uid="{554FDFA9-15BB-4B12-972E-78927D732C14}" name="Column132514" totalsRowDxfId="19"/>
+    <tableColumn id="47" xr3:uid="{4431CC4B-4ED0-4ABC-924C-91BF103A20AE}" name="Column132512" totalsRowDxfId="18"/>
+    <tableColumn id="46" xr3:uid="{6C437A0E-8A6D-4478-B7E2-0A34778B60E7}" name="Column132511" totalsRowDxfId="17"/>
+    <tableColumn id="45" xr3:uid="{9A3DF020-9578-41BA-B496-F936693A989C}" name="Column132510" totalsRowDxfId="16"/>
+    <tableColumn id="44" xr3:uid="{BC2BA275-E6CB-4DA6-8F45-9CBE680057DA}" name="Column13259" totalsRowDxfId="15"/>
+    <tableColumn id="43" xr3:uid="{35E6A8F6-ED8E-4399-825F-596EA5967F1B}" name="Column13258" totalsRowDxfId="14"/>
+    <tableColumn id="42" xr3:uid="{5104C125-2E27-4387-B9D2-F39CC14AA704}" name="Column13257" totalsRowDxfId="13"/>
+    <tableColumn id="41" xr3:uid="{8D85446A-EE97-4F1E-A08E-CC3234DCCC71}" name="Column13256" totalsRowDxfId="12"/>
+    <tableColumn id="36" xr3:uid="{786E475F-C29F-4717-950D-2E6F33ECFF47}" name="Column13255" totalsRowDxfId="11"/>
+    <tableColumn id="35" xr3:uid="{D88C32B8-F96F-492C-A956-BB09A5B161B4}" name="Column13254" totalsRowDxfId="10"/>
+    <tableColumn id="40" xr3:uid="{51BFE2E5-CC91-403A-BF9F-767E63AB3B5F}" name="Column13253" totalsRowDxfId="9"/>
+    <tableColumn id="39" xr3:uid="{668EFE9F-6816-497C-AD65-FC3F61DB685F}" name="Column13252" totalsRowDxfId="8"/>
+    <tableColumn id="37" xr3:uid="{51F3C527-95E4-43EC-873A-CE8762E66373}" name="Column1326" totalsRowDxfId="7"/>
+    <tableColumn id="34" xr3:uid="{45998420-A149-48F7-AAC3-A0986EE61766}" name="Column1324" totalsRowDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{2350E26F-CFDD-4C66-9FA4-222BE61750EC}" name="Column1323" totalsRowDxfId="5"/>
+    <tableColumn id="32" xr3:uid="{AF9F6D68-11AD-4EDC-97A2-6B8422EF708A}" name="Column1322" totalsRowDxfId="4"/>
+    <tableColumn id="31" xr3:uid="{7DAB08F1-69BD-435F-9829-3DA19CC651F9}" name="Column133" totalsRowDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{8AB5D6A3-9A8A-414C-9097-C57CEA5E3BD4}" name="Column14" totalsRowDxfId="2"/>
+    <tableColumn id="52" xr3:uid="{464C5761-13E3-41A6-A68C-D68144A91CBC}" name="Column142" totalsRowDxfId="1"/>
+    <tableColumn id="51" xr3:uid="{48056317-A43A-493F-9010-C68C0EB3735C}" name="Column15" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4AB274B9-0A1B-4F26-A207-E5383510846D}" name="Total" dataDxfId="49">
+      <calculatedColumnFormula>SUM(B2:AW2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2082,7 +2123,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B18" ca="1" si="0">RAND()</f>
-        <v>0.13693444198846549</v>
+        <v>0.60869018870668534</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -2098,7 +2139,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32777126153350888</v>
+        <v>0.29632732394776051</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -2114,7 +2155,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57640585361891561</v>
+        <v>0.87376694557192558</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -2127,7 +2168,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5888910308344395</v>
+        <v>0.50220359813973248</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -2143,7 +2184,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.175022611561365</v>
+        <v>0.94031895000110299</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -2159,7 +2200,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.4993682245761732E-2</v>
+        <v>0.43209213605323982</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -2175,7 +2216,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45326993594414999</v>
+        <v>0.94961596034591189</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -2191,7 +2232,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98000093612082251</v>
+        <v>0.89692012140771982</v>
       </c>
       <c r="C9">
         <v>80</v>
@@ -2207,7 +2248,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71975956677636921</v>
+        <v>0.407112215533739</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -2223,7 +2264,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2901195514184719</v>
+        <v>5.1556967112531549E-2</v>
       </c>
       <c r="C11">
         <v>40</v>
@@ -2239,7 +2280,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56434000247051175</v>
+        <v>0.9964756884959115</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -2255,7 +2296,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18921517907222851</v>
+        <v>0.63152749957331522</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -2271,7 +2312,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86817487514601865</v>
+        <v>5.1906562939977863E-2</v>
       </c>
       <c r="C14">
         <v>40</v>
@@ -2287,7 +2328,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96718836812319808</v>
+        <v>0.72199418317371278</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -2303,7 +2344,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1325429360683517E-2</v>
+        <v>0.41619311273656046</v>
       </c>
       <c r="C16">
         <v>25</v>
@@ -2319,7 +2360,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9496635513224159E-2</v>
+        <v>0.94002802979547906</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2334,7 +2375,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87959809618146656</v>
+        <v>0.40332354903006939</v>
       </c>
       <c r="D18" t="s">
         <v>25</v>
@@ -2350,10 +2391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62829EA8-433C-4970-81C0-C08ED68590D1}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,14 +2424,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.64629800926414294</v>
+        <f t="shared" ref="B2:B19" ca="1" si="0">RAND()</f>
+        <v>0.52567930049262812</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
@@ -2399,24 +2440,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.40265585760391598</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54657291544649456</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A17" si="0">A3+1</f>
+        <f t="shared" ref="A4:A17" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.59831229335687275</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32869247465404905</v>
       </c>
       <c r="C4" s="4">
         <v>25</v>
@@ -2427,60 +2468,60 @@
     </row>
     <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.59555341970490006</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58264531118953777</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.52600230817636118</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.780866457537154</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.55637418142846817</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49619543790152243</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.20819407311893579</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72609579601968255</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>11</v>
@@ -2491,140 +2532,140 @@
     </row>
     <row r="9" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.91595403892067884</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7.2942645335849043E-2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.73810449310557458</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18368575144043731</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.78125316430626557</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58772211890082138</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.1986318843469258</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29259438356504985</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.11266898390639346</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26012802444695982</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.90091416573345129</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4309348139716872</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.94717527321635697</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50109423598218583</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.45889841765492723</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.19721791838562142</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.1725431620145782</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99379025240415542</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>6</v>
@@ -2638,14 +2679,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <f ca="1">RAND()</f>
-        <v>0.72206491682041718</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59896187571154236</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
@@ -2653,14 +2694,40 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36326004165837089</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
         <f ca="1">RAND()</f>
-        <v>0.90018485183687569</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>25</v>
+        <v>0.6051978956090609</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <f ca="1">RAND()</f>
+        <v>0.79850219104927456</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2675,21 +2742,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A1535E-8E4E-497C-81C7-403374733E7F}">
-  <dimension ref="A1:AU16"/>
+  <dimension ref="A1:AZ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+      <selection activeCell="AX3" sqref="AX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="29" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="10.44140625" customWidth="1"/>
-    <col min="31" max="46" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="3" max="49" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="10.44140625" customWidth="1"/>
+    <col min="51" max="51" width="10.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2778,61 +2845,76 @@
         <v>85</v>
       </c>
       <c r="AD1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG1" t="s">
         <v>97</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>96</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>95</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>94</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>92</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>91</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>88</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>87</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>86</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>84</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>83</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>82</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>81</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>79</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -2854,24 +2936,33 @@
       <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AK2">
-        <v>1</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>5</v>
       </c>
       <c r="AN2">
         <v>1</v>
       </c>
+      <c r="AP2">
+        <v>1</v>
+      </c>
       <c r="AQ2">
         <v>1</v>
       </c>
-      <c r="AU2">
-        <f>SUM(B2:AT2)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AT2">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>1</v>
+      </c>
+      <c r="AZ2">
+        <f t="shared" ref="AZ2:AZ15" si="0">SUM(B2:AW2)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2914,30 +3005,42 @@
       <c r="AC3">
         <v>1</v>
       </c>
-      <c r="AI3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
         <v>2</v>
       </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
-      <c r="AR3">
-        <v>1</v>
-      </c>
-      <c r="AS3">
-        <v>1</v>
-      </c>
       <c r="AT3">
         <v>1</v>
       </c>
       <c r="AU3">
-        <f>SUM(B3:AT3)</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
+        <v>1</v>
+      </c>
+      <c r="AW3">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>1</v>
+      </c>
+      <c r="AZ3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2971,30 +3074,39 @@
       <c r="AC4">
         <v>1</v>
       </c>
-      <c r="AK4">
-        <v>1</v>
-      </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
-      <c r="AP4">
-        <v>1</v>
-      </c>
-      <c r="AR4">
+      <c r="AF4">
+        <v>4</v>
+      </c>
+      <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
         <v>2</v>
       </c>
-      <c r="AS4">
-        <v>1</v>
-      </c>
-      <c r="AT4">
-        <v>1</v>
-      </c>
-      <c r="AU4">
-        <f>SUM(B4:AT4)</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV4">
+        <v>1</v>
+      </c>
+      <c r="AW4">
+        <v>1</v>
+      </c>
+      <c r="AX4">
+        <v>2</v>
+      </c>
+      <c r="AY4">
+        <v>1</v>
+      </c>
+      <c r="AZ4">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3016,33 +3128,36 @@
       <c r="AA5">
         <v>1</v>
       </c>
-      <c r="AG5">
+      <c r="AF5">
+        <v>3</v>
+      </c>
+      <c r="AJ5">
         <v>2</v>
       </c>
-      <c r="AH5">
-        <v>1</v>
-      </c>
-      <c r="AM5">
-        <v>1</v>
-      </c>
-      <c r="AN5">
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
         <v>2</v>
       </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>1</v>
       </c>
       <c r="AS5">
         <v>1</v>
       </c>
-      <c r="AU5">
-        <f>SUM(B5:AT5)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AV5">
+        <v>1</v>
+      </c>
+      <c r="AZ5">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -3061,7 +3176,7 @@
       <c r="Z6">
         <v>1</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>1</v>
       </c>
       <c r="AG6">
@@ -3071,23 +3186,29 @@
         <v>1</v>
       </c>
       <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
         <v>2</v>
       </c>
-      <c r="AK6">
-        <v>1</v>
-      </c>
-      <c r="AP6">
-        <v>1</v>
-      </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-      <c r="AU6">
-        <f>SUM(B6:AT6)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AS6">
+        <v>1</v>
+      </c>
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AZ6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -3115,18 +3236,24 @@
       <c r="AE7">
         <v>1</v>
       </c>
-      <c r="AR7">
-        <v>1</v>
-      </c>
-      <c r="AT7">
+      <c r="AF7">
+        <v>6</v>
+      </c>
+      <c r="AH7">
         <v>1</v>
       </c>
       <c r="AU7">
-        <f>SUM(B7:AT7)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="AW7">
+        <v>1</v>
+      </c>
+      <c r="AZ7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -3154,70 +3281,85 @@
       <c r="AB8">
         <v>1</v>
       </c>
-      <c r="AL8">
-        <v>1</v>
+      <c r="AD8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>3</v>
+      </c>
+      <c r="AG8">
+        <v>2</v>
       </c>
       <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
         <v>2</v>
       </c>
-      <c r="AU8">
-        <f>SUM(B8:AT8)</f>
+      <c r="AX8">
+        <v>1</v>
+      </c>
+      <c r="AZ8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AZ9">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>18</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="Y9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <v>1</v>
-      </c>
-      <c r="AG9">
-        <v>1</v>
-      </c>
-      <c r="AH9">
-        <v>1</v>
-      </c>
-      <c r="AP9">
-        <v>1</v>
-      </c>
-      <c r="AU9">
-        <f>SUM(B9:AT9)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="T10">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
         <v>1</v>
       </c>
       <c r="AA10">
@@ -3226,18 +3368,21 @@
       <c r="AE10">
         <v>1</v>
       </c>
-      <c r="AI10">
-        <v>1</v>
-      </c>
-      <c r="AL10">
-        <v>1</v>
-      </c>
-      <c r="AU10">
-        <f>SUM(B10:AT10)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AS10">
+        <v>1</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -3253,21 +3398,21 @@
       <c r="W11">
         <v>1</v>
       </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AJ11">
+      <c r="AI11">
         <v>1</v>
       </c>
       <c r="AM11">
         <v>1</v>
       </c>
-      <c r="AU11">
-        <f>SUM(B11:AT11)</f>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+      <c r="AZ11">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3289,18 +3434,21 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="AF12">
+      <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
         <v>2</v>
       </c>
-      <c r="AI12">
-        <v>1</v>
-      </c>
-      <c r="AU12">
-        <f>SUM(B12:AT12)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -3319,36 +3467,39 @@
       <c r="R13">
         <v>1</v>
       </c>
-      <c r="AU13">
-        <f>SUM(B13:AT13)</f>
+      <c r="AX13">
+        <v>2</v>
+      </c>
+      <c r="AZ13">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="AU14">
-        <f>SUM(B14:AT14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AZ14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="AU15">
-        <f>SUM(B15:AT15)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="AZ15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
         <v>55</v>
       </c>
@@ -3400,6 +3551,11 @@
       <c r="AR16" s="5"/>
       <c r="AS16" s="5"/>
       <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
+      <c r="AV16" s="5"/>
+      <c r="AW16" s="5"/>
+      <c r="AX16" s="5"/>
+      <c r="AY16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>